<commit_message>
gui fixed till now
</commit_message>
<xml_diff>
--- a/Scripts/personDetails.xlsx
+++ b/Scripts/personDetails.xlsx
@@ -398,10 +398,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I99"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.6"/>
@@ -468,6 +468,9 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="n">
+        <v>123</v>
+      </c>
       <c r="F2" s="2" t="n"/>
       <c r="G2" s="2" t="n"/>
     </row>
@@ -549,101 +552,123 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48"/>
-    <row r="49"/>
-    <row r="50"/>
-    <row r="51"/>
-    <row r="52"/>
-    <row r="53"/>
-    <row r="54"/>
-    <row r="55"/>
-    <row r="56"/>
-    <row r="57"/>
-    <row r="58"/>
-    <row r="59"/>
-    <row r="60"/>
-    <row r="61"/>
-    <row r="62"/>
-    <row r="63"/>
-    <row r="64"/>
-    <row r="65"/>
-    <row r="66"/>
-    <row r="67"/>
-    <row r="68"/>
-    <row r="69"/>
-    <row r="70"/>
-    <row r="71"/>
-    <row r="72"/>
-    <row r="73"/>
-    <row r="74"/>
-    <row r="75"/>
-    <row r="76"/>
-    <row r="77"/>
-    <row r="78"/>
-    <row r="79"/>
-    <row r="80"/>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
-    <row r="84"/>
-    <row r="85"/>
-    <row r="86"/>
-    <row r="87"/>
-    <row r="88"/>
-    <row r="89"/>
-    <row r="90"/>
-    <row r="91"/>
-    <row r="92"/>
-    <row r="93"/>
-    <row r="94"/>
-    <row r="95"/>
-    <row r="96"/>
-    <row r="97"/>
-    <row r="98"/>
-    <row r="99"/>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>20230309Z</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>z</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>z</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>20230309X</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>20230309RA</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Raju Rastogi</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>rajuShyam</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>123123</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>123</v>
+      </c>
+      <c r="G7" t="n">
+        <v>123</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>KALTAK</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>